<commit_message>
Bugfix: AAT-5 showing null code but having part values, changing AAT-6 from xls to xlsx, re-edited README
</commit_message>
<xml_diff>
--- a/bin/constants/PartsTemplate.xlsx
+++ b/bin/constants/PartsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7672E6-873B-46AB-84AF-248D78B111FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645880-3D6B-4000-8FBD-18A0BFF78EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +63,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -101,17 +115,17 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,42 +410,43 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="21.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.5546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="3" customWidth="1"/>
+    <col min="1" max="2" width="21.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="4" customWidth="1"/>
     <col min="7" max="8" width="32.21875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="3"/>
+    <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfix: Clean up code files, updating xlsx template
</commit_message>
<xml_diff>
--- a/bin/constants/PartsTemplate.xlsx
+++ b/bin/constants/PartsTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VehicleParts\server\bin\constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645880-3D6B-4000-8FBD-18A0BFF78EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55022F7-5CDC-4814-A4BA-B11BECB7C673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <cols>
     <col min="1" max="2" width="21.109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="25.5546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="4" customWidth="1"/>
     <col min="7" max="8" width="32.21875" style="4" customWidth="1"/>

</xml_diff>